<commit_message>
Update figure 4️⃣ code for publication
</commit_message>
<xml_diff>
--- a/_Code/Fig4/tables/Histone_PTMs_metadata.xlsx
+++ b/_Code/Fig4/tables/Histone_PTMs_metadata.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niar/OneDrive - CRG - Centre de Regulacio Genomica/Suz12_AS_project/_Code/Fig3/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\narecco\OneDrive - CRG - Centre de Regulacio Genomica\Suz12_AS_project\_Code\Fig4\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FEEF34-F024-6A4B-B596-C33E479089CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24500" yWindow="2020" windowWidth="24740" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24495" yWindow="2025" windowWidth="24735" windowHeight="15000" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Form" sheetId="1" r:id="rId1"/>
+    <sheet name="DIA" sheetId="1" r:id="rId1"/>
+    <sheet name="DDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11_39_14" localSheetId="0">Form!$A$1:$E$2</definedName>
+    <definedName name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11_39_14" localSheetId="1">DDA!$A$1:$E$2</definedName>
+    <definedName name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11_39_14" localSheetId="0">DIA!$A$1:$E$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,8 +35,20 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11 39 14" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11 39 14" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="/Users/niar/OneDrive - CRG - Centre de Regulacio Genomica/Suz12_AS_project/15_Histone_PTMs/FullSet2/ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11 39 14.csv" decimal="," thousands="." comma="1" qualifier="none">
+      <textFields count="6">
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11 39 141" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="/Users/niar/OneDrive - CRG - Centre de Regulacio Genomica/Suz12_AS_project/15_Histone_PTMs/FullSet2/ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11 39 14.csv" decimal="," thousands="." comma="1" qualifier="none">
       <textFields count="6">
         <textField type="text"/>
@@ -51,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -101,9 +114,6 @@
     <t>2022MH003_NIAR_004_02_30pto_DIA</t>
   </si>
   <si>
-    <t>2022MH003_NIAR_005_02__30pto_DIA</t>
-  </si>
-  <si>
     <t>2022MH003_NIAR_006_02_30pto_DIA</t>
   </si>
   <si>
@@ -240,13 +250,70 @@
   </si>
   <si>
     <t>Proteomic_Facility_FileName</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_001_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_002_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_003_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_004_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_005_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_006_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_007_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_008_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MZ006_IVMO_009_02_25pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_005_02_30pto_DIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022MH003_NIAR_001_01_30pto_DDA                                                                                                  </t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_003_01_30pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_002_01_30pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_004_01_30pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_005_01_30pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_006_01_30pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_007_01_30pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_008_01_30pto_DDA</t>
+  </si>
+  <si>
+    <t>2022MH003_NIAR_009_01_30pto_DDA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -287,7 +354,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -303,7 +370,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11 39 14" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11 39 14" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ListPTM_quantification_of_histones___A._Pilot_experiment_0_2022_06_29_11 39 14" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,26 +673,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.625" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -633,307 +706,649 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>45</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
       <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
         <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
       <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
         <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
-        <v>56</v>
-      </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
-        <v>59</v>
-      </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="40.125" customWidth="1"/>
+    <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
       </c>
       <c r="E19">
         <v>3</v>

</xml_diff>